<commit_message>
Data corr. (cities names)
</commit_message>
<xml_diff>
--- a/migforecasting/cities10/1/d9.xlsx
+++ b/migforecasting/cities10/1/d9.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Albert\.spyder-py3\ITMO-2\migforecasting\cities10\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,14 +20,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="93">
-  <si>
-    <t>Орехово-
-Зуево</t>
-  </si>
-  <si>
-    <t>Электро-
-сталь</t>
-  </si>
   <si>
     <t>ПОКАЗАТЕЛИ</t>
   </si>
@@ -419,6 +411,12 @@
       </rPr>
       <t>14)</t>
     </r>
+  </si>
+  <si>
+    <t>Электросталь</t>
+  </si>
+  <si>
+    <t>Орехово-Зуево</t>
   </si>
 </sst>
 </file>
@@ -842,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AK25" sqref="AK25"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,94 +916,94 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R2" t="s">
+        <v>92</v>
+      </c>
+      <c r="S2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="T2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y2" t="s">
         <v>13</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Z2" t="s">
         <v>13</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" t="s">
         <v>14</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
         <v>14</v>
       </c>
-      <c r="W2" t="s">
-        <v>18</v>
-      </c>
-      <c r="X2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="AC2" t="s">
         <v>15</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AD2" t="s">
         <v>15</v>
       </c>
-      <c r="AA2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>17</v>
-      </c>
       <c r="AE2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="AF2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -1108,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO4" s="3"/>
     </row>
@@ -1117,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7">
         <v>216.7</v>
@@ -1216,7 +1214,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7">
         <v>13.9</v>
@@ -1315,7 +1313,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7">
         <v>14.1</v>
@@ -1414,7 +1412,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7">
         <v>-0.2</v>
@@ -1688,7 +1686,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="7">
         <v>4592</v>
@@ -1786,7 +1784,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1824,7 +1822,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="7">
         <v>31</v>
@@ -1922,13 +1920,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E17" s="7">
         <v>318</v>
@@ -2020,7 +2018,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="7">
         <v>793</v>
@@ -2118,7 +2116,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -2156,7 +2154,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="7">
         <v>26820</v>
@@ -2254,7 +2252,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="7">
         <v>8214</v>
@@ -2296,7 +2294,7 @@
         <v>9003</v>
       </c>
       <c r="P21" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q21" s="7">
         <v>7738</v>
@@ -2352,7 +2350,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7">
         <v>43.9</v>
@@ -2394,7 +2392,7 @@
         <v>30.7</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="7">
         <v>36.200000000000003</v>
@@ -2450,7 +2448,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="7">
         <v>23.2</v>
@@ -2507,10 +2505,10 @@
         <v>28.6</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="V23" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="W23" s="7">
         <v>29.3</v>
@@ -2531,10 +2529,10 @@
         <v>30.8</v>
       </c>
       <c r="AC23" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AD23" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AE23" s="7">
         <v>20.8</v>
@@ -2548,7 +2546,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="7">
         <v>42</v>
@@ -2646,7 +2644,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -2684,7 +2682,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="7">
         <v>6.9</v>
@@ -2782,7 +2780,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" s="7">
         <v>6.2</v>
@@ -2880,7 +2878,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -2918,7 +2916,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" s="7">
         <v>797</v>
@@ -3016,7 +3014,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="7">
         <v>36.799999999999997</v>
@@ -3114,7 +3112,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -3152,7 +3150,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C32" s="7">
         <v>1412</v>
@@ -3250,7 +3248,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" s="7">
         <v>65.2</v>
@@ -3349,7 +3347,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" s="7">
         <v>6</v>
@@ -3448,7 +3446,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -3487,7 +3485,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C36" s="7">
         <v>2.1</v>
@@ -3586,7 +3584,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C37" s="7">
         <v>96.9</v>
@@ -3685,7 +3683,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="7">
         <v>13</v>
@@ -3784,7 +3782,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -3823,7 +3821,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C40" s="7">
         <v>5.5</v>
@@ -3922,7 +3920,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C41" s="7">
         <v>254.8</v>
@@ -4021,19 +4019,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E42" s="7">
         <v>1317</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G42" s="7">
         <v>1559</v>
@@ -4084,10 +4082,10 @@
         <v>1145</v>
       </c>
       <c r="W42" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X42" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y42" s="10">
         <v>875</v>
@@ -4120,19 +4118,19 @@
         <v>41</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E43" s="7">
         <v>537</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G43" s="7">
         <v>697</v>
@@ -4183,10 +4181,10 @@
         <v>419</v>
       </c>
       <c r="W43" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X43" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y43" s="10">
         <v>341</v>
@@ -4219,7 +4217,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -4258,7 +4256,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45" s="7">
         <v>33846</v>
@@ -4357,7 +4355,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C46" s="7">
         <v>3286</v>
@@ -4456,7 +4454,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47" s="7">
         <v>38</v>
@@ -4555,7 +4553,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48" s="7">
         <v>10.4</v>
@@ -4654,7 +4652,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
@@ -4693,7 +4691,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50" s="7">
         <v>5461</v>
@@ -4792,7 +4790,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -4831,7 +4829,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
@@ -4870,31 +4868,31 @@
         <v>51</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K53" s="7">
         <v>3</v>
@@ -4903,40 +4901,40 @@
         <v>5</v>
       </c>
       <c r="M53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="V53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="W53" s="10">
         <v>1</v>
       </c>
       <c r="X53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y53" s="10">
         <v>1</v>
@@ -4945,10 +4943,10 @@
         <v>1</v>
       </c>
       <c r="AA53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AC53" s="10">
         <v>3</v>
@@ -4957,7 +4955,7 @@
         <v>2</v>
       </c>
       <c r="AE53" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AF53" s="10">
         <v>1</v>
@@ -4969,7 +4967,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C54" s="7">
         <v>33</v>
@@ -5068,7 +5066,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C55" s="7">
         <v>9</v>
@@ -5167,7 +5165,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -5206,31 +5204,31 @@
         <v>55</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K57" s="7">
         <v>153.30000000000001</v>
@@ -5239,64 +5237,64 @@
         <v>192.5</v>
       </c>
       <c r="M57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N57" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O57" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="V57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="W57" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="X57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y57" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Z57" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AC57" s="10">
         <v>284.2</v>
       </c>
       <c r="AD57" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AE57" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AF57" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.25">
@@ -5305,7 +5303,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C58" s="7">
         <v>14944.1</v>
@@ -5404,7 +5402,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C59" s="7">
         <v>6117.4</v>
@@ -5503,7 +5501,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
@@ -5542,7 +5540,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C61" s="7">
         <v>345.5</v>
@@ -5614,7 +5612,7 @@
         <v>23</v>
       </c>
       <c r="Z61" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AA61" s="10">
         <v>1582.5</v>
@@ -5641,7 +5639,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -5680,7 +5678,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C63" s="7">
         <v>396.2</v>
@@ -5779,7 +5777,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C64" s="7">
         <v>6409</v>
@@ -5878,16 +5876,16 @@
         <v>63</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D65" s="7">
         <v>370</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F65" s="7">
         <v>160</v>
@@ -5899,34 +5897,34 @@
         <v>125</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O65" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S65" s="10">
         <v>495</v>
@@ -5938,19 +5936,19 @@
         <v>120</v>
       </c>
       <c r="V65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="W65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="X65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Z65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AA65" s="10">
         <v>275</v>
@@ -5959,16 +5957,16 @@
         <v>355</v>
       </c>
       <c r="AC65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AD65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AE65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AF65" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
@@ -6088,7 +6086,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
@@ -6127,7 +6125,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C70" s="7">
         <v>16442.7</v>
@@ -6226,7 +6224,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C71" s="10">
         <v>132.69999999999999</v>
@@ -6295,7 +6293,7 @@
         <v>100</v>
       </c>
       <c r="Y71" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z71" s="7">
         <v>110</v>
@@ -6325,7 +6323,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C72" s="10">
         <v>504.4</v>
@@ -6424,10 +6422,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D73" s="10">
         <v>104.7</v>
@@ -6439,7 +6437,7 @@
         <v>115</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H73" s="10">
         <v>150.6</v>
@@ -6451,7 +6449,7 @@
         <v>139.6</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L73" s="10">
         <v>113.6</v>
@@ -6463,37 +6461,37 @@
         <v>106.3</v>
       </c>
       <c r="O73" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P73" s="7">
         <v>117.3</v>
       </c>
       <c r="Q73" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="R73" s="7">
         <v>106</v>
       </c>
       <c r="S73" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="T73" s="7">
         <v>113.6</v>
       </c>
       <c r="U73" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="V73" s="7">
         <v>140.5</v>
       </c>
       <c r="W73" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X73" s="7">
         <v>94.4</v>
       </c>
       <c r="Y73" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z73" s="7">
         <v>124.8</v>
@@ -6505,7 +6503,7 @@
         <v>115.2</v>
       </c>
       <c r="AC73" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AD73" s="7">
         <v>112</v>
@@ -6523,7 +6521,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
@@ -6562,7 +6560,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C75" s="10">
         <v>1550.5</v>
@@ -6661,7 +6659,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C76" s="10">
         <v>24.1</v>
@@ -6742,10 +6740,10 @@
         <v>10.5</v>
       </c>
       <c r="AC76" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AD76" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AE76" s="7">
         <v>1.5</v>
@@ -6760,7 +6758,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C77" s="10">
         <v>16.7</v>
@@ -6799,10 +6797,10 @@
         <v>10.9</v>
       </c>
       <c r="O77" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P77" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q77" s="7">
         <v>9.1999999999999993</v>
@@ -6841,10 +6839,10 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="AC77" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AD77" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AE77" s="7">
         <v>0.4</v>
@@ -6855,7 +6853,7 @@
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B78" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>